<commit_message>
(+)    reorg w/header.js, menu/js, with util.js updates
</commit_message>
<xml_diff>
--- a/Test/Logo Slide.xlsx
+++ b/Test/Logo Slide.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Brief</t>
   </si>
@@ -157,6 +157,27 @@
   </si>
   <si>
     <t>Enters to Home screen immediate</t>
+  </si>
+  <si>
+    <t>Test Vectors</t>
+  </si>
+  <si>
+    <t>1. From idle S1-&gt;S2-&gt;S2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     first slide, then no more logo updates</t>
+  </si>
+  <si>
+    <t>*currently H-&gt;E-&gt;E works fine</t>
+  </si>
+  <si>
+    <t>*H-&gt;S-&gt;S works fine</t>
+  </si>
+  <si>
+    <t>*H-&gt;E-&gt;S is not</t>
+  </si>
+  <si>
+    <t>logo moves farther right &amp; gets bigger? Do console prints to check</t>
   </si>
 </sst>
 </file>
@@ -520,7 +541,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -632,30 +653,53 @@
       <c r="A14" t="s">
         <v>9</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>